<commit_message>
Spreadsheet updated to represent N in scientific notation
</commit_message>
<xml_diff>
--- a/Erastothenes/Erastothenes.xlsx
+++ b/Erastothenes/Erastothenes.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevi\Source\Repos\MathsAlgorithms\Erastothenes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevi\source\repos\MathsAlgorithms\Erastothenes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3AF48B-B5D1-4F89-870A-BBF6DBEDCCED}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9F00CF-17CB-4EF6-96C5-FD6F4570AF03}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24576" windowHeight="9396" activeTab="2" xr2:uid="{8D1779FE-3953-428B-B9C0-D8ABCFEB7B16}"/>
   </bookViews>
   <sheets>
-    <sheet name="100000" sheetId="1" r:id="rId1"/>
-    <sheet name="1000000" sheetId="2" r:id="rId2"/>
-    <sheet name="dyn array" sheetId="3" r:id="rId3"/>
+    <sheet name="1.00E+05&lt;=N&lt;=2.00E+06" sheetId="1" r:id="rId1"/>
+    <sheet name="1.00E+06&lt;=N&lt;=2.00E+07" sheetId="2" r:id="rId2"/>
+    <sheet name="1.00E+08&lt;=N&lt;=2.00E+09" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -79,7 +79,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -94,6 +94,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -191,7 +192,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100000'!$B$1</c:f>
+              <c:f>'1.00E+05&lt;=N&lt;=2.00E+06'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -214,9 +215,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'100000'!$A$2:$A$21</c:f>
+              <c:f>'1.00E+05&lt;=N&lt;=2.00E+06'!$A$2:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>100000</c:v>
@@ -283,7 +284,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'100000'!$B$2:$B$21</c:f>
+              <c:f>'1.00E+05&lt;=N&lt;=2.00E+06'!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
@@ -376,7 +377,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -639,7 +640,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1000000'!$B$1</c:f>
+              <c:f>'1.00E+06&lt;=N&lt;=2.00E+07'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -662,9 +663,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'1000000'!$A$2:$A$21</c:f>
+              <c:f>'1.00E+06&lt;=N&lt;=2.00E+07'!$A$2:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1000000</c:v>
@@ -731,7 +732,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1000000'!$B$2:$B$21</c:f>
+              <c:f>'1.00E+06&lt;=N&lt;=2.00E+07'!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
@@ -824,7 +825,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1045,6 +1046,15 @@
               <a:t>Running time of the Sieve of Erastothenes</a:t>
             </a:r>
           </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>(using dynamic array allocation)</a:t>
+            </a:r>
+          </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
@@ -1087,7 +1097,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'dyn array'!$B$1</c:f>
+              <c:f>'1.00E+08&lt;=N&lt;=2.00E+09'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1110,9 +1120,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'dyn array'!$A$2:$A$21</c:f>
+              <c:f>'1.00E+08&lt;=N&lt;=2.00E+09'!$A$2:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>100000000</c:v>
@@ -1179,7 +1189,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'dyn array'!$B$2:$B$21</c:f>
+              <c:f>'1.00E+08&lt;=N&lt;=2.00E+09'!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1272,7 +1282,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3551,7 +3561,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3572,7 +3582,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="6">
         <v>100000</v>
       </c>
       <c r="B2" s="1">
@@ -3584,7 +3594,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="6">
         <f>A2+$A$2</f>
         <v>200000</v>
       </c>
@@ -3597,7 +3607,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="6">
         <f t="shared" ref="A4:A21" si="0">A3+$A$2</f>
         <v>300000</v>
       </c>
@@ -3610,7 +3620,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
@@ -3623,7 +3633,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
@@ -3636,7 +3646,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>600000</v>
       </c>
@@ -3649,7 +3659,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
@@ -3662,7 +3672,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>800000</v>
       </c>
@@ -3675,7 +3685,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>900000</v>
       </c>
@@ -3688,7 +3698,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
@@ -3701,7 +3711,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>1100000</v>
       </c>
@@ -3714,7 +3724,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>1200000</v>
       </c>
@@ -3727,7 +3737,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>1300000</v>
       </c>
@@ -3740,7 +3750,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>1400000</v>
       </c>
@@ -3753,7 +3763,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
@@ -3766,7 +3776,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>1600000</v>
       </c>
@@ -3779,7 +3789,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>1700000</v>
       </c>
@@ -3792,7 +3802,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>1800000</v>
       </c>
@@ -3805,7 +3815,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>1900000</v>
       </c>
@@ -3818,7 +3828,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>2000000</v>
       </c>
@@ -3843,7 +3853,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3860,7 +3870,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="6">
         <v>1000000</v>
       </c>
       <c r="B2" s="1">
@@ -3872,7 +3882,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="6">
         <f>A2+$A$2</f>
         <v>2000000</v>
       </c>
@@ -3885,7 +3895,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="6">
         <f t="shared" ref="A4:A21" si="0">A3+$A$2</f>
         <v>3000000</v>
       </c>
@@ -3898,7 +3908,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>4000000</v>
       </c>
@@ -3911,7 +3921,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>5000000</v>
       </c>
@@ -3924,7 +3934,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>6000000</v>
       </c>
@@ -3937,7 +3947,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>7000000</v>
       </c>
@@ -3950,7 +3960,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>8000000</v>
       </c>
@@ -3963,7 +3973,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>9000000</v>
       </c>
@@ -3976,7 +3986,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
@@ -3989,7 +3999,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>11000000</v>
       </c>
@@ -4002,7 +4012,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>12000000</v>
       </c>
@@ -4015,7 +4025,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>13000000</v>
       </c>
@@ -4028,7 +4038,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>14000000</v>
       </c>
@@ -4041,7 +4051,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>15000000</v>
       </c>
@@ -4054,7 +4064,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>16000000</v>
       </c>
@@ -4067,7 +4077,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>17000000</v>
       </c>
@@ -4080,7 +4090,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>18000000</v>
       </c>
@@ -4093,7 +4103,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>19000000</v>
       </c>
@@ -4106,7 +4116,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>20000000</v>
       </c>
@@ -4130,7 +4140,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4151,7 +4161,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="6">
         <v>100000000</v>
       </c>
       <c r="B2" s="1">
@@ -4163,7 +4173,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="6">
         <f>A2+$A$2</f>
         <v>200000000</v>
       </c>
@@ -4176,20 +4186,20 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <f t="shared" ref="A4:A51" si="0">A3+$A$2</f>
+      <c r="A4" s="6">
+        <f t="shared" ref="A4:A21" si="0">A3+$A$2</f>
         <v>300000000</v>
       </c>
       <c r="B4" s="1">
         <v>5161</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C51" si="1">B4/$B$2</f>
+        <f t="shared" ref="C4:C21" si="1">B4/$B$2</f>
         <v>3.2893562778840026</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>400000000</v>
       </c>
@@ -4202,7 +4212,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>500000000</v>
       </c>
@@ -4215,7 +4225,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>600000000</v>
       </c>
@@ -4228,7 +4238,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>700000000</v>
       </c>
@@ -4241,7 +4251,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>800000000</v>
       </c>
@@ -4254,7 +4264,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>900000000</v>
       </c>
@@ -4267,7 +4277,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>1000000000</v>
       </c>
@@ -4280,7 +4290,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>1100000000</v>
       </c>
@@ -4293,7 +4303,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>1200000000</v>
       </c>
@@ -4306,7 +4316,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>1300000000</v>
       </c>
@@ -4319,7 +4329,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>1400000000</v>
       </c>
@@ -4332,7 +4342,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>1500000000</v>
       </c>
@@ -4345,7 +4355,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>1600000000</v>
       </c>
@@ -4358,7 +4368,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>1700000000</v>
       </c>
@@ -4371,7 +4381,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>1800000000</v>
       </c>
@@ -4384,7 +4394,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>1900000000</v>
       </c>
@@ -4397,7 +4407,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>2000000000</v>
       </c>

</xml_diff>